<commit_message>
Qiasi formulas added, some changes have been made to main watum
</commit_message>
<xml_diff>
--- a/WATUM_v0.2/Dx_2017_Noori_et_al_Paper02_severn.xlsx
+++ b/WATUM_v0.2/Dx_2017_Noori_et_al_Paper02_severn.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="63900" windowWidth="14805" windowHeight="7335" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="63900" windowWidth="14805" windowHeight="7335" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Setting" sheetId="8" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="سورن سفارش نوری" sheetId="13" state="hidden" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_ftn1" localSheetId="4">'hidden tab'!$P$24</definedName>
+    <definedName name="_ftn1" localSheetId="4">'hidden tab'!#REF!</definedName>
     <definedName name="Delta_T__seconds">Setting!$B$10</definedName>
     <definedName name="Delta_X">Setting!$H$10:$H$17</definedName>
     <definedName name="Delta_X__meters">Setting!$B$9</definedName>
@@ -105,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="116">
   <si>
     <t>Project Name</t>
   </si>
@@ -447,6 +447,12 @@
   </si>
   <si>
     <t>Noori et al (2017)</t>
+  </si>
+  <si>
+    <t>Qiasi 01 (2017)</t>
+  </si>
+  <si>
+    <t>Qiasi 02 (2017)</t>
   </si>
 </sst>
 </file>
@@ -456,7 +462,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="41" x14ac:knownFonts="1">
+  <fonts count="40" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -704,14 +710,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1337,7 +1335,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="44">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1381,7 +1379,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1560,45 +1557,45 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="30" xfId="37" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="37" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="37" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="37" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="36" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="37" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="37" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="37" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="37" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="37" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="37" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="37" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="37" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="37" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="37" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1609,28 +1606,22 @@
     <xf numFmtId="164" fontId="20" fillId="32" borderId="7" xfId="37" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="43" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="39" borderId="12" xfId="37" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="39" borderId="7" xfId="37" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="39" borderId="7" xfId="37" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="39" borderId="7" xfId="37" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
@@ -1647,8 +1638,14 @@
     <xf numFmtId="0" fontId="34" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="44">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="2" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="3" builtinId="38" customBuiltin="1"/>
@@ -1682,7 +1679,6 @@
     <cellStyle name="Heading 2" xfId="31" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="32" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="33" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8"/>
     <cellStyle name="Input" xfId="34" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="35" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="36" builtinId="28" customBuiltin="1"/>
@@ -2690,6 +2686,72 @@
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
     <mruColors>
       <color rgb="FFFBB39D"/>
       <color rgb="FFCC99FF"/>
@@ -4363,7 +4425,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="C0C0C0"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -4812,7 +4874,7 @@
       </c>
       <c r="B6" s="45" t="str">
         <f ca="1">LEFT(CELL("filename"),FIND("[",CELL("filename"),1)-1)</f>
-        <v>C:\Users\Mostafa\Desktop\watum_Working_Branch\WATUM_v0.2\</v>
+        <v>C:\Users\Mostafa\Documents\GitHub\watum\WATUM_v0.2\</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -7031,7 +7093,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="LDC is not permitted to be blanked">
           <x14:formula1>
-            <xm:f>'hidden tab'!$P$2:$P$22</xm:f>
+            <xm:f>'hidden tab'!$P$2:$P$24</xm:f>
           </x14:formula1>
           <xm:sqref>B11</xm:sqref>
         </x14:dataValidation>
@@ -7164,7 +7226,7 @@
       <c r="W1" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="87" t="s">
+      <c r="X1" s="85" t="s">
         <v>108</v>
       </c>
       <c r="Y1" s="14" t="s">
@@ -7215,10 +7277,10 @@
       <c r="AN1" s="60" t="s">
         <v>79</v>
       </c>
-      <c r="AO1" s="90" t="s">
+      <c r="AO1" s="88" t="s">
         <v>106</v>
       </c>
-      <c r="AP1" s="90" t="s">
+      <c r="AP1" s="88" t="s">
         <v>107</v>
       </c>
     </row>
@@ -7291,7 +7353,7 @@
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/1000</f>
         <v>0.21</v>
       </c>
-      <c r="X2" s="88">
+      <c r="X2" s="86">
         <v>1.0510314000000001</v>
       </c>
       <c r="Y2" s="71" t="str">
@@ -7356,11 +7418,11 @@
       <c r="AN2" s="70">
         <v>0</v>
       </c>
-      <c r="AO2" s="91">
+      <c r="AO2" s="89">
         <f>FLOOR(Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters,1)</f>
         <v>6</v>
       </c>
-      <c r="AP2" s="91">
+      <c r="AP2" s="89">
         <f>((1/1000000)*Table1[[#This Row],[Cup]]*Table1[[#This Row],[R ratio]]*Table1[[#This Row],[Inj Mass]])/Table1[[#This Row],[Q '[m3/sec']]]</f>
         <v>0</v>
       </c>
@@ -7434,7 +7496,7 @@
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/1000</f>
         <v>1.175</v>
       </c>
-      <c r="X3" s="88">
+      <c r="X3" s="86">
         <v>0.22527449999999999</v>
       </c>
       <c r="Y3" s="71" t="str">
@@ -7499,11 +7561,11 @@
       <c r="AN3" s="70">
         <v>1</v>
       </c>
-      <c r="AO3" s="91">
+      <c r="AO3" s="89">
         <f>FLOOR(Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters,1)</f>
         <v>33</v>
       </c>
-      <c r="AP3" s="91">
+      <c r="AP3" s="89">
         <f>((1/1000000)*Table1[[#This Row],[Cup]]*Table1[[#This Row],[R ratio]]*Table1[[#This Row],[Inj Mass]])/Table1[[#This Row],[Q '[m3/sec']]]</f>
         <v>0</v>
       </c>
@@ -7577,7 +7639,7 @@
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/1000</f>
         <v>2.875</v>
       </c>
-      <c r="X4" s="89">
+      <c r="X4" s="87">
         <v>0.11053590000000001</v>
       </c>
       <c r="Y4" s="71" t="str">
@@ -7638,11 +7700,11 @@
         <v>1.1333</v>
       </c>
       <c r="AN4" s="70"/>
-      <c r="AO4" s="91">
+      <c r="AO4" s="89">
         <f>FLOOR(Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters,1)</f>
         <v>82</v>
       </c>
-      <c r="AP4" s="91">
+      <c r="AP4" s="89">
         <f>((1/1000000)*Table1[[#This Row],[Cup]]*Table1[[#This Row],[R ratio]]*Table1[[#This Row],[Inj Mass]])/Table1[[#This Row],[Q '[m3/sec']]]</f>
         <v>0</v>
       </c>
@@ -7716,7 +7778,7 @@
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/1000</f>
         <v>5.2750000000000004</v>
       </c>
-      <c r="X5" s="89">
+      <c r="X5" s="87">
         <v>5.8002699999999997E-2</v>
       </c>
       <c r="Y5" s="71" t="str">
@@ -7777,11 +7839,11 @@
         <v>2.4666999999999999</v>
       </c>
       <c r="AN5" s="70"/>
-      <c r="AO5" s="91">
+      <c r="AO5" s="89">
         <f>FLOOR(Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters,1)</f>
         <v>150</v>
       </c>
-      <c r="AP5" s="91">
+      <c r="AP5" s="89">
         <f>((1/1000000)*Table1[[#This Row],[Cup]]*Table1[[#This Row],[R ratio]]*Table1[[#This Row],[Inj Mass]])/Table1[[#This Row],[Q '[m3/sec']]]</f>
         <v>0</v>
       </c>
@@ -7855,7 +7917,7 @@
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/1000</f>
         <v>7.7750000000000004</v>
       </c>
-      <c r="X6" s="89">
+      <c r="X6" s="87">
         <v>3.4605400000000001E-2</v>
       </c>
       <c r="Y6" s="71" t="str">
@@ -7916,11 +7978,11 @@
         <v>3.7332999999999998</v>
       </c>
       <c r="AN6" s="70"/>
-      <c r="AO6" s="91">
+      <c r="AO6" s="89">
         <f>FLOOR(Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters,1)</f>
         <v>222</v>
       </c>
-      <c r="AP6" s="91">
+      <c r="AP6" s="89">
         <f>((1/1000000)*Table1[[#This Row],[Cup]]*Table1[[#This Row],[R ratio]]*Table1[[#This Row],[Inj Mass]])/Table1[[#This Row],[Q '[m3/sec']]]</f>
         <v>0</v>
       </c>
@@ -7994,7 +8056,7 @@
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/1000</f>
         <v>10.275</v>
       </c>
-      <c r="X7" s="89">
+      <c r="X7" s="87">
         <v>2.1080000000000002E-2</v>
       </c>
       <c r="Y7" s="71" t="str">
@@ -8055,11 +8117,11 @@
         <v>5.0332999999999997</v>
       </c>
       <c r="AN7" s="70"/>
-      <c r="AO7" s="91">
+      <c r="AO7" s="89">
         <f>FLOOR(Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters,1)</f>
         <v>293</v>
       </c>
-      <c r="AP7" s="91">
+      <c r="AP7" s="89">
         <f>((1/1000000)*Table1[[#This Row],[Cup]]*Table1[[#This Row],[R ratio]]*Table1[[#This Row],[Inj Mass]])/Table1[[#This Row],[Q '[m3/sec']]]</f>
         <v>0</v>
       </c>
@@ -8133,7 +8195,7 @@
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/1000</f>
         <v>13.775</v>
       </c>
-      <c r="X8" s="89">
+      <c r="X8" s="87">
         <v>2.0655E-2</v>
       </c>
       <c r="Y8" s="71" t="str">
@@ -8194,11 +8256,11 @@
         <v>6.5369000000000002</v>
       </c>
       <c r="AN8" s="70"/>
-      <c r="AO8" s="91">
+      <c r="AO8" s="89">
         <f>FLOOR(Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters,1)</f>
         <v>393</v>
       </c>
-      <c r="AP8" s="91">
+      <c r="AP8" s="89">
         <f>((1/1000000)*Table1[[#This Row],[Cup]]*Table1[[#This Row],[R ratio]]*Table1[[#This Row],[Inj Mass]])/Table1[[#This Row],[Q '[m3/sec']]]</f>
         <v>0</v>
       </c>
@@ -8400,13 +8462,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.5703125" style="94" customWidth="1"/>
+    <col min="1" max="1" width="2.5703125" style="92" customWidth="1"/>
     <col min="2" max="7" width="2.5703125" customWidth="1"/>
     <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
     <col min="9" max="15" width="2.28515625" customWidth="1"/>
@@ -8414,89 +8476,89 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="92"/>
+      <c r="A1" s="90"/>
       <c r="H1">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="92"/>
+      <c r="A2" s="90"/>
       <c r="H2">
         <v>5</v>
       </c>
-      <c r="P2" t="s">
+      <c r="P2" s="96" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="92"/>
+      <c r="A3" s="90"/>
       <c r="H3">
         <v>10</v>
       </c>
-      <c r="P3" t="s">
+      <c r="P3" s="96" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="92"/>
+      <c r="A4" s="90"/>
       <c r="H4">
         <v>25</v>
       </c>
-      <c r="P4" t="s">
+      <c r="P4" s="96" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="92"/>
+      <c r="A5" s="90"/>
       <c r="H5">
         <v>50</v>
       </c>
-      <c r="P5" t="s">
+      <c r="P5" s="96" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="92"/>
+      <c r="A6" s="90"/>
       <c r="H6">
         <v>100</v>
       </c>
-      <c r="P6" t="s">
+      <c r="P6" s="96" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="92"/>
+      <c r="A7" s="90"/>
       <c r="H7">
         <v>150</v>
       </c>
-      <c r="P7" t="s">
+      <c r="P7" s="96" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="93"/>
+      <c r="A8" s="91"/>
       <c r="H8">
         <v>200</v>
       </c>
-      <c r="P8" t="s">
+      <c r="P8" s="96" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="92"/>
+      <c r="A9" s="90"/>
       <c r="H9">
         <v>250</v>
       </c>
-      <c r="P9" t="s">
+      <c r="P9" s="96" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="93"/>
+      <c r="A10" s="91"/>
       <c r="H10">
         <v>300</v>
       </c>
-      <c r="P10" t="s">
+      <c r="P10" s="96" t="s">
         <v>90</v>
       </c>
     </row>
@@ -8504,7 +8566,7 @@
       <c r="H11">
         <v>350</v>
       </c>
-      <c r="P11" t="s">
+      <c r="P11" s="96" t="s">
         <v>109</v>
       </c>
     </row>
@@ -8512,7 +8574,7 @@
       <c r="H12">
         <v>400</v>
       </c>
-      <c r="P12" t="s">
+      <c r="P12" s="96" t="s">
         <v>110</v>
       </c>
     </row>
@@ -8520,7 +8582,7 @@
       <c r="H13">
         <v>450</v>
       </c>
-      <c r="P13" t="s">
+      <c r="P13" s="96" t="s">
         <v>111</v>
       </c>
     </row>
@@ -8528,7 +8590,7 @@
       <c r="H14">
         <v>500</v>
       </c>
-      <c r="P14" t="s">
+      <c r="P14" s="96" t="s">
         <v>91</v>
       </c>
     </row>
@@ -8536,7 +8598,7 @@
       <c r="H15">
         <v>550</v>
       </c>
-      <c r="P15" t="s">
+      <c r="P15" s="96" t="s">
         <v>92</v>
       </c>
     </row>
@@ -8544,7 +8606,7 @@
       <c r="H16">
         <v>600</v>
       </c>
-      <c r="P16" t="s">
+      <c r="P16" s="96" t="s">
         <v>93</v>
       </c>
     </row>
@@ -8552,7 +8614,7 @@
       <c r="H17">
         <v>650</v>
       </c>
-      <c r="P17" t="s">
+      <c r="P17" s="96" t="s">
         <v>94</v>
       </c>
     </row>
@@ -8560,7 +8622,7 @@
       <c r="H18">
         <v>700</v>
       </c>
-      <c r="P18" t="s">
+      <c r="P18" s="96" t="s">
         <v>95</v>
       </c>
     </row>
@@ -8568,7 +8630,7 @@
       <c r="H19">
         <v>750</v>
       </c>
-      <c r="P19" t="s">
+      <c r="P19" s="96" t="s">
         <v>96</v>
       </c>
     </row>
@@ -8576,7 +8638,7 @@
       <c r="H20">
         <v>800</v>
       </c>
-      <c r="P20" t="s">
+      <c r="P20" s="96" t="s">
         <v>112</v>
       </c>
     </row>
@@ -8584,7 +8646,7 @@
       <c r="H21">
         <v>900</v>
       </c>
-      <c r="P21" t="s">
+      <c r="P21" s="96" t="s">
         <v>113</v>
       </c>
     </row>
@@ -8592,24 +8654,28 @@
       <c r="H22">
         <v>1000</v>
       </c>
-      <c r="P22" t="s">
-        <v>104</v>
+      <c r="P22" s="96" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="23" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H23">
         <v>1250</v>
       </c>
-      <c r="P23" s="84"/>
+      <c r="P23" s="97" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="24" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H24">
         <v>1500</v>
       </c>
-      <c r="P24" s="85"/>
+      <c r="P24" s="96" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="25" spans="8:16" x14ac:dyDescent="0.25">
-      <c r="P25" s="86"/>
+      <c r="P25" s="84"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -8641,7 +8707,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:S8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:S8"/>
     </sheetView>
   </sheetViews>
@@ -9472,15 +9538,15 @@
     </row>
     <row r="28" spans="6:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F28" s="39"/>
-      <c r="G28" s="95" t="s">
+      <c r="G28" s="93" t="s">
         <v>82</v>
       </c>
-      <c r="H28" s="96"/>
-      <c r="I28" s="96"/>
-      <c r="J28" s="96"/>
-      <c r="K28" s="96"/>
-      <c r="L28" s="96"/>
-      <c r="M28" s="97"/>
+      <c r="H28" s="94"/>
+      <c r="I28" s="94"/>
+      <c r="J28" s="94"/>
+      <c r="K28" s="94"/>
+      <c r="L28" s="94"/>
+      <c r="M28" s="95"/>
     </row>
     <row r="29" spans="6:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F29" s="40" t="s">

</xml_diff>

<commit_message>
After first run, when curvature added.
xlsx file modified, and with the first Ghiasi-Noori Ex formula, model ran.
</commit_message>
<xml_diff>
--- a/WATUM_v0.2/Dx_2017_Noori_et_al_Paper02_severn.xlsx
+++ b/WATUM_v0.2/Dx_2017_Noori_et_al_Paper02_severn.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="63900" windowWidth="14805" windowHeight="7335" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="63900" windowWidth="14805" windowHeight="7335" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Setting" sheetId="8" r:id="rId1"/>
@@ -105,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="117">
   <si>
     <t>Project Name</t>
   </si>
@@ -453,6 +453,9 @@
   </si>
   <si>
     <t>Qiasi 02 (2017)</t>
+  </si>
+  <si>
+    <t>Curvature (sigma)</t>
   </si>
 </sst>
 </file>
@@ -462,7 +465,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="40" x14ac:knownFonts="1">
+  <fonts count="42" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -735,6 +738,17 @@
       <color theme="1"/>
       <name val="Cutive Mono"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Cutive Mono"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Consolas"/>
     </font>
   </fonts>
   <fills count="40">
@@ -1380,7 +1394,7 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1629,6 +1643,18 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="7" xfId="37" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="35" borderId="7" xfId="37" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1637,12 +1663,6 @@
     </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1690,7 +1710,31 @@
     <cellStyle name="Total" xfId="40" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="41" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="45">
+  <dxfs count="46">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Cutive Mono"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -4327,91 +4371,92 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:AP8" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43" tableBorderDxfId="42" headerRowCellStyle="Note" dataCellStyle="Note">
-  <autoFilter ref="A1:AP8"/>
-  <tableColumns count="42">
-    <tableColumn id="1" name="Name" dataDxfId="41"/>
-    <tableColumn id="2" name="Start point distance [meters]" dataDxfId="40"/>
-    <tableColumn id="3" name="End Point distance  [meters]" dataDxfId="39" dataCellStyle="Note"/>
-    <tableColumn id="4" name="Q [m3/sec]" dataDxfId="38"/>
-    <tableColumn id="5" name="Ti" dataDxfId="37" dataCellStyle="Note"/>
-    <tableColumn id="6" name="Tp" dataDxfId="36"/>
-    <tableColumn id="7" name="Tt" dataDxfId="35" dataCellStyle="Note"/>
-    <tableColumn id="8" name="Q average" dataDxfId="34" dataCellStyle="Note"/>
-    <tableColumn id="9" name="Drainage Area [km2]" dataDxfId="33" dataCellStyle="Note"/>
-    <tableColumn id="10" name="longitudinal slope" dataDxfId="32"/>
-    <tableColumn id="11" name="depth [meters]" dataDxfId="31"/>
-    <tableColumn id="12" name="width [meters]" dataDxfId="30"/>
-    <tableColumn id="13" name="Cup" dataDxfId="29"/>
-    <tableColumn id="14" name="Inj Mass" dataDxfId="28" dataCellStyle="Note"/>
-    <tableColumn id="15" name="R ratio" dataDxfId="27" dataCellStyle="Note"/>
-    <tableColumn id="16" name="Ref" dataDxfId="26" dataCellStyle="Note"/>
-    <tableColumn id="17" name="Calculated Velocity [meters/sec]" dataDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:AQ8" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44" tableBorderDxfId="43" headerRowCellStyle="Note" dataCellStyle="Note">
+  <autoFilter ref="A1:AQ8"/>
+  <tableColumns count="43">
+    <tableColumn id="1" name="Name" dataDxfId="42"/>
+    <tableColumn id="2" name="Start point distance [meters]" dataDxfId="41"/>
+    <tableColumn id="3" name="End Point distance  [meters]" dataDxfId="40" dataCellStyle="Note"/>
+    <tableColumn id="4" name="Q [m3/sec]" dataDxfId="39"/>
+    <tableColumn id="5" name="Ti" dataDxfId="38" dataCellStyle="Note"/>
+    <tableColumn id="6" name="Tp" dataDxfId="37"/>
+    <tableColumn id="7" name="Tt" dataDxfId="36" dataCellStyle="Note"/>
+    <tableColumn id="8" name="Q average" dataDxfId="35" dataCellStyle="Note"/>
+    <tableColumn id="9" name="Drainage Area [km2]" dataDxfId="34" dataCellStyle="Note"/>
+    <tableColumn id="10" name="longitudinal slope" dataDxfId="33"/>
+    <tableColumn id="11" name="depth [meters]" dataDxfId="32"/>
+    <tableColumn id="12" name="width [meters]" dataDxfId="31"/>
+    <tableColumn id="13" name="Cup" dataDxfId="30"/>
+    <tableColumn id="14" name="Inj Mass" dataDxfId="29" dataCellStyle="Note"/>
+    <tableColumn id="15" name="R ratio" dataDxfId="28" dataCellStyle="Note"/>
+    <tableColumn id="16" name="Ref" dataDxfId="27" dataCellStyle="Note"/>
+    <tableColumn id="17" name="Calculated Velocity [meters/sec]" dataDxfId="26">
       <calculatedColumnFormula>Table1[Q '[m3/sec']]/(Table1[depth '[meters']]*Table1[width '[meters']])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" name="calculated time [hours]" dataDxfId="24" dataCellStyle="Note">
+    <tableColumn id="18" name="calculated time [hours]" dataDxfId="25" dataCellStyle="Note">
       <calculatedColumnFormula>(Table1[[#This Row],[Reach Length '[meters']]]/(Table1[[#This Row],[Q '[m3/sec']]]/(Table1[[#This Row],[depth '[meters']]]*Table1[[#This Row],[width '[meters']]])))/3600</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" name="Observed Velocity [meters / seconds]" dataDxfId="23" dataCellStyle="Note">
+    <tableColumn id="19" name="Observed Velocity [meters / seconds]" dataDxfId="24" dataCellStyle="Note">
       <calculatedColumnFormula>(Table1[[#This Row],[End Point distance  '[meters']]]/(3600*Table1[[#This Row],[Tp]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" name="ɳ" dataDxfId="22"/>
-    <tableColumn id="21" name="river side slope" dataDxfId="21"/>
-    <tableColumn id="22" name="Initial Concentration [mgr/Lit]" dataDxfId="20"/>
-    <tableColumn id="23" name="End Point of Reach [km]" dataDxfId="19" dataCellStyle="Note">
+    <tableColumn id="20" name="ɳ" dataDxfId="23"/>
+    <tableColumn id="21" name="river side slope" dataDxfId="22"/>
+    <tableColumn id="22" name="Initial Concentration [mgr/Lit]" dataDxfId="21"/>
+    <tableColumn id="23" name="End Point of Reach [km]" dataDxfId="20" dataCellStyle="Note">
       <calculatedColumnFormula>Table1[[#This Row],[End Point distance  '[meters']]]/1000</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="24" name="Only Observed Concentration (if you had losses and want to use formula look @ AP column) PPM" dataDxfId="18"/>
-    <tableColumn id="25" name="Error in Calc time Vs Obs Time" dataDxfId="17" dataCellStyle="Percent">
+    <tableColumn id="24" name="Only Observed Concentration (if you had losses and want to use formula look @ AP column) PPM" dataDxfId="19"/>
+    <tableColumn id="25" name="Error in Calc time Vs Obs Time" dataDxfId="18" dataCellStyle="Percent">
       <calculatedColumnFormula>IF(AVERAGE(Table1[[#This Row],[Error Ti]]&lt;=AVERAGE(Table1[[#This Row],[Error Tp]])),"use Ti","use Tp")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="26" name="Reach Length [meters]" dataDxfId="16" dataCellStyle="Note">
+    <tableColumn id="26" name="Reach Length [meters]" dataDxfId="17" dataCellStyle="Note">
       <calculatedColumnFormula>Table1[[#This Row],[End Point distance  '[meters']]]-Table1[[#This Row],[Start point distance '[meters']]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="39" name="Reach Time (seconds)" dataDxfId="15" dataCellStyle="Note">
+    <tableColumn id="39" name="Reach Time (seconds)" dataDxfId="16" dataCellStyle="Note">
       <calculatedColumnFormula>(Table1[[#This Row],[Tp]]-AN2)*3600</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" name="Time Cell" dataDxfId="14" dataCellStyle="Note">
+    <tableColumn id="27" name="Time Cell" dataDxfId="15" dataCellStyle="Note">
       <calculatedColumnFormula>FLOOR((Table1[[#This Row],[Tp]]*3600)/Table1[[#This Row],[Delta T]],1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="37" name="End Spatial Cell" dataDxfId="13" dataCellStyle="Note">
+    <tableColumn id="37" name="End Spatial Cell" dataDxfId="14" dataCellStyle="Note">
       <calculatedColumnFormula>Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="38" name="Start Spatial Cell" dataDxfId="12" dataCellStyle="Note">
+    <tableColumn id="38" name="Start Spatial Cell" dataDxfId="13" dataCellStyle="Note">
       <calculatedColumnFormula>Table1[[#This Row],[Start point distance '[meters']]]/Delta_X__meters</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="28" name="Delta T" dataDxfId="11" dataCellStyle="Note">
+    <tableColumn id="28" name="Delta T" dataDxfId="12" dataCellStyle="Note">
       <calculatedColumnFormula>Delta_T__seconds</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="29" name="Error Ti" dataDxfId="10" dataCellStyle="Percent">
+    <tableColumn id="29" name="Error Ti" dataDxfId="11" dataCellStyle="Percent">
       <calculatedColumnFormula>((Table1[[#This Row],[Ti]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Ti]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="30" name="Error Tp" dataDxfId="9" dataCellStyle="Percent">
+    <tableColumn id="30" name="Error Tp" dataDxfId="10" dataCellStyle="Percent">
       <calculatedColumnFormula>(('Reach Propertise'!$F2-'Reach Propertise'!$R2)/'Reach Propertise'!$F2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="31" name="Error Tt" dataDxfId="8" dataCellStyle="Percent">
+    <tableColumn id="31" name="Error Tt" dataDxfId="9" dataCellStyle="Percent">
       <calculatedColumnFormula>((Table1[[#This Row],[Tt]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Tt]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="32" name="Column1" dataDxfId="7" dataCellStyle="Percent">
+    <tableColumn id="32" name="Column1" dataDxfId="8" dataCellStyle="Percent">
       <calculatedColumnFormula>Table1[[#This Row],[width '[meters']]]/Table1[[#This Row],[depth '[meters']]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="33" name="Vi" dataDxfId="6" dataCellStyle="Note">
+    <tableColumn id="33" name="Vi" dataDxfId="7" dataCellStyle="Note">
       <calculatedColumnFormula>Table1[[#This Row],[depth '[meters']]]*Table1[[#This Row],[width '[meters']]]*Delta_X__meters</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="34" name="delta Tp" dataDxfId="5" dataCellStyle="Note">
+    <tableColumn id="34" name="delta Tp" dataDxfId="6" dataCellStyle="Note">
       <calculatedColumnFormula>Table1[[#This Row],[Column3]]-Table1[[#This Row],[Column2]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="35" name="Column2" dataDxfId="4" dataCellStyle="Note"/>
-    <tableColumn id="36" name="Column3" dataDxfId="3" dataCellStyle="Note">
+    <tableColumn id="35" name="Column2" dataDxfId="5" dataCellStyle="Note"/>
+    <tableColumn id="36" name="Column3" dataDxfId="4" dataCellStyle="Note">
       <calculatedColumnFormula>'Reach Propertise'!$F2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="40" name="Column4" dataDxfId="2" dataCellStyle="Note"/>
-    <tableColumn id="41" name="X cells for evaluation and comparison with obsered" dataDxfId="1" dataCellStyle="Note">
+    <tableColumn id="40" name="Column4" dataDxfId="3" dataCellStyle="Note"/>
+    <tableColumn id="41" name="X cells for evaluation and comparison with obsered" dataDxfId="2" dataCellStyle="Note">
       <calculatedColumnFormula>FLOOR(Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="42" name="Observed Concentration [ppm] using formula2" dataDxfId="0" dataCellStyle="Note">
+    <tableColumn id="42" name="Observed Concentration [ppm] using formula2" dataDxfId="1" dataCellStyle="Note">
       <calculatedColumnFormula>((1/1000000)*Table1[[#This Row],[Cup]]*Table1[[#This Row],[R ratio]]*Table1[[#This Row],[Inj Mass]])/Table1[[#This Row],[Q '[m3/sec']]]</calculatedColumnFormula>
     </tableColumn>
+    <tableColumn id="43" name="Curvature (sigma)" dataDxfId="0" dataCellStyle="Note"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5018,7 +5063,7 @@
         <v>7</v>
       </c>
       <c r="B11" s="48" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
@@ -7108,11 +7153,11 @@
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:AP11"/>
+  <dimension ref="A1:AQ11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="AM1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
+      <selection pane="bottomLeft" activeCell="AQ8" sqref="AQ8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7156,7 +7201,7 @@
     <col min="43" max="16384" width="9.140625" style="57"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" s="61" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:43" s="61" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>39</v>
       </c>
@@ -7283,8 +7328,11 @@
       <c r="AP1" s="88" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="2" spans="1:42" s="70" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AQ1" s="96" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:43" s="70" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="65" t="s">
         <v>97</v>
       </c>
@@ -7426,8 +7474,11 @@
         <f>((1/1000000)*Table1[[#This Row],[Cup]]*Table1[[#This Row],[R ratio]]*Table1[[#This Row],[Inj Mass]])/Table1[[#This Row],[Q '[m3/sec']]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:42" s="74" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AQ2" s="95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:43" s="74" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="65" t="s">
         <v>98</v>
       </c>
@@ -7569,8 +7620,11 @@
         <f>((1/1000000)*Table1[[#This Row],[Cup]]*Table1[[#This Row],[R ratio]]*Table1[[#This Row],[Inj Mass]])/Table1[[#This Row],[Q '[m3/sec']]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:42" s="74" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AQ3" s="95">
+        <v>1.1759999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:43" s="74" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="75" t="s">
         <v>99</v>
       </c>
@@ -7708,8 +7762,11 @@
         <f>((1/1000000)*Table1[[#This Row],[Cup]]*Table1[[#This Row],[R ratio]]*Table1[[#This Row],[Inj Mass]])/Table1[[#This Row],[Q '[m3/sec']]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:42" s="74" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AQ4" s="95">
+        <v>1.228</v>
+      </c>
+    </row>
+    <row r="5" spans="1:43" s="74" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="75" t="s">
         <v>100</v>
       </c>
@@ -7847,8 +7904,11 @@
         <f>((1/1000000)*Table1[[#This Row],[Cup]]*Table1[[#This Row],[R ratio]]*Table1[[#This Row],[Inj Mass]])/Table1[[#This Row],[Q '[m3/sec']]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:42" s="74" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AQ5" s="95">
+        <v>1.1379999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:43" s="74" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="75" t="s">
         <v>101</v>
       </c>
@@ -7986,8 +8046,11 @@
         <f>((1/1000000)*Table1[[#This Row],[Cup]]*Table1[[#This Row],[R ratio]]*Table1[[#This Row],[Inj Mass]])/Table1[[#This Row],[Q '[m3/sec']]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:42" s="74" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AQ6" s="95">
+        <v>1.0449999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:43" s="74" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="75" t="s">
         <v>102</v>
       </c>
@@ -8125,8 +8188,11 @@
         <f>((1/1000000)*Table1[[#This Row],[Cup]]*Table1[[#This Row],[R ratio]]*Table1[[#This Row],[Inj Mass]])/Table1[[#This Row],[Q '[m3/sec']]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:42" s="74" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AQ7" s="95">
+        <v>1.173</v>
+      </c>
+    </row>
+    <row r="8" spans="1:43" s="74" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="75" t="s">
         <v>103</v>
       </c>
@@ -8264,16 +8330,19 @@
         <f>((1/1000000)*Table1[[#This Row],[Cup]]*Table1[[#This Row],[R ratio]]*Table1[[#This Row],[Inj Mass]])/Table1[[#This Row],[Q '[m3/sec']]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:42" s="80" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AQ8" s="95">
+        <v>1.6439999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:43" s="80" customFormat="1" x14ac:dyDescent="0.25">
       <c r="X9" s="81"/>
       <c r="Y9" s="82"/>
     </row>
-    <row r="10" spans="1:42" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:43" s="80" customFormat="1" x14ac:dyDescent="0.25">
       <c r="X10" s="81"/>
       <c r="Y10" s="82"/>
     </row>
-    <row r="11" spans="1:42" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:43" s="62" customFormat="1" x14ac:dyDescent="0.25">
       <c r="X11" s="63"/>
       <c r="Y11" s="64"/>
     </row>
@@ -8462,7 +8531,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
+    <sheetView topLeftCell="B13" workbookViewId="0">
       <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
@@ -8486,7 +8555,7 @@
       <c r="H2">
         <v>5</v>
       </c>
-      <c r="P2" s="96" t="s">
+      <c r="P2" s="93" t="s">
         <v>105</v>
       </c>
     </row>
@@ -8495,7 +8564,7 @@
       <c r="H3">
         <v>10</v>
       </c>
-      <c r="P3" s="96" t="s">
+      <c r="P3" s="93" t="s">
         <v>83</v>
       </c>
     </row>
@@ -8504,7 +8573,7 @@
       <c r="H4">
         <v>25</v>
       </c>
-      <c r="P4" s="96" t="s">
+      <c r="P4" s="93" t="s">
         <v>84</v>
       </c>
     </row>
@@ -8513,7 +8582,7 @@
       <c r="H5">
         <v>50</v>
       </c>
-      <c r="P5" s="96" t="s">
+      <c r="P5" s="93" t="s">
         <v>85</v>
       </c>
     </row>
@@ -8522,7 +8591,7 @@
       <c r="H6">
         <v>100</v>
       </c>
-      <c r="P6" s="96" t="s">
+      <c r="P6" s="93" t="s">
         <v>86</v>
       </c>
     </row>
@@ -8531,7 +8600,7 @@
       <c r="H7">
         <v>150</v>
       </c>
-      <c r="P7" s="96" t="s">
+      <c r="P7" s="93" t="s">
         <v>87</v>
       </c>
     </row>
@@ -8540,7 +8609,7 @@
       <c r="H8">
         <v>200</v>
       </c>
-      <c r="P8" s="96" t="s">
+      <c r="P8" s="93" t="s">
         <v>88</v>
       </c>
     </row>
@@ -8549,7 +8618,7 @@
       <c r="H9">
         <v>250</v>
       </c>
-      <c r="P9" s="96" t="s">
+      <c r="P9" s="93" t="s">
         <v>89</v>
       </c>
     </row>
@@ -8558,7 +8627,7 @@
       <c r="H10">
         <v>300</v>
       </c>
-      <c r="P10" s="96" t="s">
+      <c r="P10" s="93" t="s">
         <v>90</v>
       </c>
     </row>
@@ -8566,7 +8635,7 @@
       <c r="H11">
         <v>350</v>
       </c>
-      <c r="P11" s="96" t="s">
+      <c r="P11" s="93" t="s">
         <v>109</v>
       </c>
     </row>
@@ -8574,7 +8643,7 @@
       <c r="H12">
         <v>400</v>
       </c>
-      <c r="P12" s="96" t="s">
+      <c r="P12" s="93" t="s">
         <v>110</v>
       </c>
     </row>
@@ -8582,7 +8651,7 @@
       <c r="H13">
         <v>450</v>
       </c>
-      <c r="P13" s="96" t="s">
+      <c r="P13" s="93" t="s">
         <v>111</v>
       </c>
     </row>
@@ -8590,7 +8659,7 @@
       <c r="H14">
         <v>500</v>
       </c>
-      <c r="P14" s="96" t="s">
+      <c r="P14" s="93" t="s">
         <v>91</v>
       </c>
     </row>
@@ -8598,7 +8667,7 @@
       <c r="H15">
         <v>550</v>
       </c>
-      <c r="P15" s="96" t="s">
+      <c r="P15" s="93" t="s">
         <v>92</v>
       </c>
     </row>
@@ -8606,7 +8675,7 @@
       <c r="H16">
         <v>600</v>
       </c>
-      <c r="P16" s="96" t="s">
+      <c r="P16" s="93" t="s">
         <v>93</v>
       </c>
     </row>
@@ -8614,7 +8683,7 @@
       <c r="H17">
         <v>650</v>
       </c>
-      <c r="P17" s="96" t="s">
+      <c r="P17" s="93" t="s">
         <v>94</v>
       </c>
     </row>
@@ -8622,7 +8691,7 @@
       <c r="H18">
         <v>700</v>
       </c>
-      <c r="P18" s="96" t="s">
+      <c r="P18" s="93" t="s">
         <v>95</v>
       </c>
     </row>
@@ -8630,7 +8699,7 @@
       <c r="H19">
         <v>750</v>
       </c>
-      <c r="P19" s="96" t="s">
+      <c r="P19" s="93" t="s">
         <v>96</v>
       </c>
     </row>
@@ -8638,7 +8707,7 @@
       <c r="H20">
         <v>800</v>
       </c>
-      <c r="P20" s="96" t="s">
+      <c r="P20" s="93" t="s">
         <v>112</v>
       </c>
     </row>
@@ -8646,7 +8715,7 @@
       <c r="H21">
         <v>900</v>
       </c>
-      <c r="P21" s="96" t="s">
+      <c r="P21" s="93" t="s">
         <v>113</v>
       </c>
     </row>
@@ -8654,7 +8723,7 @@
       <c r="H22">
         <v>1000</v>
       </c>
-      <c r="P22" s="96" t="s">
+      <c r="P22" s="93" t="s">
         <v>114</v>
       </c>
     </row>
@@ -8662,7 +8731,7 @@
       <c r="H23">
         <v>1250</v>
       </c>
-      <c r="P23" s="97" t="s">
+      <c r="P23" s="94" t="s">
         <v>115</v>
       </c>
     </row>
@@ -8670,7 +8739,7 @@
       <c r="H24">
         <v>1500</v>
       </c>
-      <c r="P24" s="96" t="s">
+      <c r="P24" s="93" t="s">
         <v>104</v>
       </c>
     </row>
@@ -8705,425 +8774,467 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:S8"/>
+  <dimension ref="A1:U7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:S8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:U7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>0.68015664268852827</v>
+      </c>
+      <c r="B1">
+        <v>28625.050200190482</v>
+      </c>
+      <c r="C1">
+        <v>7.5719455818316364E-2</v>
+      </c>
+      <c r="D1">
+        <v>14.381730614658528</v>
+      </c>
+      <c r="E1">
+        <v>8397713719.6893826</v>
+      </c>
+      <c r="F1">
+        <v>16659637699.36138</v>
+      </c>
+      <c r="G1">
+        <v>53.346954629423969</v>
+      </c>
+      <c r="H1">
+        <v>24.944368285190407</v>
+      </c>
+      <c r="I1">
+        <v>8.9633660700929063</v>
+      </c>
+      <c r="J1">
+        <v>1.7314104976385134</v>
+      </c>
+      <c r="K1">
+        <v>27.52928439270714</v>
+      </c>
+      <c r="L1">
+        <v>15.313694228549927</v>
+      </c>
+      <c r="M1">
+        <v>41.108331001401368</v>
+      </c>
+      <c r="N1">
+        <v>27.453400050271661</v>
+      </c>
+      <c r="O1">
+        <v>5.4214850129549559</v>
+      </c>
+      <c r="P1">
+        <v>35.884936034862996</v>
+      </c>
+      <c r="Q1">
+        <v>9.014130288461315</v>
+      </c>
+      <c r="R1">
+        <v>21.676550151409781</v>
+      </c>
+      <c r="S1">
+        <v>13.942155495606716</v>
+      </c>
+      <c r="T1">
+        <v>6.3665901299092251</v>
+      </c>
+      <c r="U1">
+        <v>9.9604329875250084</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>0.68015664268852827</v>
+        <v>0.31322849740396147</v>
       </c>
       <c r="B2">
-        <v>28625.050200190482</v>
+        <v>68852.677170974173</v>
       </c>
       <c r="C2">
-        <v>7.5719455818316364E-2</v>
+        <v>0.12293688374554616</v>
       </c>
       <c r="D2">
-        <v>14.381730614658528</v>
+        <v>36.525382552168367</v>
       </c>
       <c r="E2">
-        <v>8397713719.6893826</v>
+        <v>1191998690413.3914</v>
       </c>
       <c r="F2">
-        <v>16659637699.36138</v>
+        <v>1694556080269.5063</v>
       </c>
       <c r="G2">
-        <v>53.346954629423969</v>
+        <v>32.534000789767745</v>
       </c>
       <c r="H2">
-        <v>24.944368285190407</v>
+        <v>33.417506117698331</v>
       </c>
       <c r="I2">
-        <v>8.9633660700929063</v>
+        <v>11.715853656867665</v>
       </c>
       <c r="J2">
-        <v>1.7314104976385134</v>
+        <v>1.0141777360050148</v>
       </c>
       <c r="K2">
-        <v>27.52928439270714</v>
+        <v>38.84840735065351</v>
       </c>
       <c r="L2">
-        <v>15.313694228549927</v>
+        <v>23.277590695310806</v>
       </c>
       <c r="M2">
-        <v>41.108331001401368</v>
+        <v>116.47353178631496</v>
       </c>
       <c r="N2">
-        <v>27.453400050271661</v>
+        <v>34.811568463568335</v>
       </c>
       <c r="O2">
-        <v>5.4214850129549559</v>
+        <v>10.147704164784699</v>
       </c>
       <c r="P2">
-        <v>35.884936034862996</v>
+        <v>32.643688089241856</v>
       </c>
       <c r="Q2">
-        <v>9.014130288461315</v>
+        <v>5.1609111854629521</v>
       </c>
       <c r="R2">
-        <v>21.676550151409781</v>
+        <v>20.812053037658316</v>
       </c>
       <c r="S2">
-        <v>13.942155495606716</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+        <v>16.388113959583489</v>
+      </c>
+      <c r="T2">
+        <v>15.507373328494982</v>
+      </c>
+      <c r="U2">
+        <v>18.266370598192992</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>0.31322849740396147</v>
+        <v>0.26698111766955995</v>
       </c>
       <c r="B3">
-        <v>68852.677170974173</v>
+        <v>39274.013348111286</v>
       </c>
       <c r="C3">
-        <v>0.12293688374554616</v>
+        <v>0.29774150721407944</v>
       </c>
       <c r="D3">
-        <v>36.525382552168367</v>
+        <v>33.390806589551822</v>
       </c>
       <c r="E3">
-        <v>1191998690413.3914</v>
+        <v>12738920.171506403</v>
       </c>
       <c r="F3">
-        <v>1694556080269.5063</v>
+        <v>14182975.825430201</v>
       </c>
       <c r="G3">
-        <v>32.534000789767745</v>
+        <v>14.03880466851562</v>
       </c>
       <c r="H3">
-        <v>33.417506117698331</v>
+        <v>43.206819882737427</v>
       </c>
       <c r="I3">
-        <v>11.715853656867665</v>
+        <v>9.9525069786968974</v>
       </c>
       <c r="J3">
-        <v>1.0141777360050148</v>
+        <v>0.48228789072402922</v>
       </c>
       <c r="K3">
-        <v>38.84840735065351</v>
+        <v>45.241875502440102</v>
       </c>
       <c r="L3">
-        <v>23.277590695310806</v>
+        <v>41.63305266191491</v>
       </c>
       <c r="M3">
-        <v>116.47353178631496</v>
+        <v>276.74217753538369</v>
       </c>
       <c r="N3">
-        <v>34.811568463568335</v>
+        <v>35.359440679528277</v>
       </c>
       <c r="O3">
-        <v>10.147704164784699</v>
+        <v>65535</v>
       </c>
       <c r="P3">
-        <v>32.643688089241856</v>
+        <v>31.962756249979922</v>
       </c>
       <c r="Q3">
-        <v>5.1609111854629521</v>
+        <v>3.4118064406572564</v>
       </c>
       <c r="R3">
-        <v>20.812053037658316</v>
+        <v>23.866176447391744</v>
       </c>
       <c r="S3">
-        <v>16.388113959583489</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+        <v>15.377687775050815</v>
+      </c>
+      <c r="T3">
+        <v>17.67255234581512</v>
+      </c>
+      <c r="U3">
+        <v>21.947416391384401</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>0.26698111766955995</v>
+        <v>0.35933783316164253</v>
       </c>
       <c r="B4">
-        <v>39274.013348111286</v>
+        <v>64026.44107621452</v>
       </c>
       <c r="C4">
-        <v>0.29774150721407944</v>
+        <v>0.2196960007178472</v>
       </c>
       <c r="D4">
-        <v>33.390806589551822</v>
+        <v>20.372935049446575</v>
       </c>
       <c r="E4">
-        <v>12738920.171506403</v>
+        <v>11660815.389813524</v>
       </c>
       <c r="F4">
-        <v>14182975.825430201</v>
+        <v>15746001.233835166</v>
       </c>
       <c r="G4">
-        <v>14.03880466851562</v>
+        <v>18.624112795831529</v>
       </c>
       <c r="H4">
-        <v>43.206819882737427</v>
+        <v>33.314135015728112</v>
       </c>
       <c r="I4">
-        <v>9.9525069786968974</v>
+        <v>8.3248995491209179</v>
       </c>
       <c r="J4">
-        <v>0.48228789072402922</v>
+        <v>0.62146782257943423</v>
       </c>
       <c r="K4">
-        <v>45.241875502440102</v>
+        <v>35.177546386489475</v>
       </c>
       <c r="L4">
-        <v>41.63305266191491</v>
+        <v>28.096184267128709</v>
       </c>
       <c r="M4">
-        <v>276.74217753538369</v>
+        <v>131.99859525068348</v>
       </c>
       <c r="N4">
-        <v>35.359440679528277</v>
+        <v>29.10676961852668</v>
       </c>
       <c r="O4">
-        <v>65535</v>
+        <v>149551654.81536677</v>
       </c>
       <c r="P4">
-        <v>31.962756249979922</v>
+        <v>30.806528017469848</v>
       </c>
       <c r="Q4">
-        <v>3.4118064406572564</v>
+        <v>4.3379828015827844</v>
       </c>
       <c r="R4">
-        <v>23.866176447391744</v>
+        <v>23.551261448561682</v>
       </c>
       <c r="S4">
-        <v>15.377687775050815</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+        <v>13.278955923320112</v>
+      </c>
+      <c r="T4">
+        <v>10.741242534297676</v>
+      </c>
+      <c r="U4">
+        <v>15.009172570217011</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>0.35933783316164253</v>
+        <v>0.34387364708602081</v>
       </c>
       <c r="B5">
-        <v>64026.44107621452</v>
+        <v>9147441664.3559856</v>
       </c>
       <c r="C5">
-        <v>0.2196960007178472</v>
+        <v>0.16127039307728611</v>
       </c>
       <c r="D5">
-        <v>20.372935049446575</v>
+        <v>77.369606165605788</v>
       </c>
       <c r="E5">
-        <v>11660815.389813524</v>
+        <v>1.9290048029375352E+18</v>
       </c>
       <c r="F5">
-        <v>15746001.233835166</v>
+        <v>2.801819736520597E+18</v>
       </c>
       <c r="G5">
-        <v>18.624112795831529</v>
+        <v>62.363966507937029</v>
       </c>
       <c r="H5">
-        <v>33.314135015728112</v>
+        <v>43.443566400056703</v>
       </c>
       <c r="I5">
-        <v>8.3248995491209179</v>
+        <v>19.802115942320338</v>
       </c>
       <c r="J5">
-        <v>0.62146782257943423</v>
+        <v>1.4626982397490671</v>
       </c>
       <c r="K5">
-        <v>35.177546386489475</v>
+        <v>51.712553908003869</v>
       </c>
       <c r="L5">
-        <v>28.096184267128709</v>
+        <v>26.791796370902254</v>
       </c>
       <c r="M5">
-        <v>131.99859525068348</v>
+        <v>141.35315939797886</v>
       </c>
       <c r="N5">
-        <v>29.10676961852668</v>
+        <v>51.744233499347608</v>
       </c>
       <c r="O5">
-        <v>149551654.81536677</v>
+        <v>18.279787512399285</v>
       </c>
       <c r="P5">
-        <v>30.806528017469848</v>
+        <v>43.34296430768245</v>
       </c>
       <c r="Q5">
-        <v>4.3379828015827844</v>
+        <v>7.3080205694117195</v>
       </c>
       <c r="R5">
-        <v>23.551261448561682</v>
+        <v>33.465758842333642</v>
       </c>
       <c r="S5">
-        <v>13.278955923320112</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+        <v>24.85729790564373</v>
+      </c>
+      <c r="T5">
+        <v>18.288122515136749</v>
+      </c>
+      <c r="U5">
+        <v>20.168816904604935</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>0.34387364708602081</v>
+        <v>0.33506683054146424</v>
       </c>
       <c r="B6">
-        <v>9147441664.3559856</v>
+        <v>621158150.54461765</v>
       </c>
       <c r="C6">
-        <v>0.16127039307728611</v>
+        <v>0.10442477316346464</v>
       </c>
       <c r="D6">
-        <v>77.369606165605788</v>
+        <v>60.174042250514447</v>
       </c>
       <c r="E6">
-        <v>1.9290048029375352E+18</v>
+        <v>2.2739472572257246E+20</v>
       </c>
       <c r="F6">
-        <v>2.801819736520597E+18</v>
+        <v>3.6764427167066312E+20</v>
       </c>
       <c r="G6">
-        <v>62.363966507937029</v>
+        <v>70.772994369132917</v>
       </c>
       <c r="H6">
-        <v>43.443566400056703</v>
+        <v>33.197199515206243</v>
       </c>
       <c r="I6">
-        <v>19.802115942320338</v>
+        <v>17.026340576566227</v>
       </c>
       <c r="J6">
-        <v>1.4626982397490671</v>
+        <v>1.6960669498047289</v>
       </c>
       <c r="K6">
-        <v>51.712553908003869</v>
+        <v>41.144595726212735</v>
       </c>
       <c r="L6">
-        <v>26.791796370902254</v>
+        <v>18.926217222075252</v>
       </c>
       <c r="M6">
-        <v>141.35315939797886</v>
+        <v>84.482643114858618</v>
       </c>
       <c r="N6">
-        <v>51.744233499347608</v>
+        <v>42.521834635580191</v>
       </c>
       <c r="O6">
-        <v>18.279787512399285</v>
+        <v>1.3901698702784904</v>
       </c>
       <c r="P6">
-        <v>43.34296430768245</v>
+        <v>37.450196851082339</v>
       </c>
       <c r="Q6">
-        <v>7.3080205694117195</v>
+        <v>7.4357658243047737</v>
       </c>
       <c r="R6">
-        <v>33.465758842333642</v>
+        <v>27.08994181247148</v>
       </c>
       <c r="S6">
-        <v>24.85729790564373</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+        <v>21.067085368232753</v>
+      </c>
+      <c r="T6">
+        <v>20.055271029640178</v>
+      </c>
+      <c r="U6">
+        <v>20.826456333325456</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>0.33506683054146424</v>
+        <v>0.45280611092443795</v>
       </c>
       <c r="B7">
-        <v>621158150.54461765</v>
+        <v>2723227.9512344319</v>
       </c>
       <c r="C7">
-        <v>0.10442477316346464</v>
+        <v>0.17333530579880232</v>
       </c>
       <c r="D7">
-        <v>60.174042250514447</v>
+        <v>27.460498428617271</v>
       </c>
       <c r="E7">
-        <v>2.2739472572257246E+20</v>
+        <v>7078511204.2171917</v>
       </c>
       <c r="F7">
-        <v>3.6764427167066312E+20</v>
+        <v>10784896704.219383</v>
       </c>
       <c r="G7">
-        <v>70.772994369132917</v>
+        <v>35.458238134848095</v>
       </c>
       <c r="H7">
-        <v>33.197199515206243</v>
+        <v>35.26734159215561</v>
       </c>
       <c r="I7">
-        <v>17.026340576566227</v>
+        <v>11.227535573950105</v>
       </c>
       <c r="J7">
-        <v>1.6960669498047289</v>
+        <v>1.0291592446967921</v>
       </c>
       <c r="K7">
-        <v>41.144595726212735</v>
+        <v>39.998500617030622</v>
       </c>
       <c r="L7">
-        <v>18.926217222075252</v>
+        <v>25.0441175460994</v>
       </c>
       <c r="M7">
-        <v>84.482643114858618</v>
+        <v>103.21750311087098</v>
       </c>
       <c r="N7">
-        <v>42.521834635580191</v>
+        <v>35.320773438636586</v>
       </c>
       <c r="O7">
-        <v>1.3901698702784904</v>
+        <v>-6.9202824218865526</v>
       </c>
       <c r="P7">
-        <v>37.450196851082339</v>
+        <v>37.394201405106315</v>
       </c>
       <c r="Q7">
-        <v>7.4357658243047737</v>
+        <v>6.422533260982461</v>
       </c>
       <c r="R7">
-        <v>27.08994181247148</v>
+        <v>28.194582095621172</v>
       </c>
       <c r="S7">
-        <v>21.067085368232753</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>0.45280611092443795</v>
-      </c>
-      <c r="B8">
-        <v>2723227.9512344319</v>
-      </c>
-      <c r="C8">
-        <v>0.17333530579880232</v>
-      </c>
-      <c r="D8">
-        <v>27.460498428617271</v>
-      </c>
-      <c r="E8">
-        <v>7078511204.2171917</v>
-      </c>
-      <c r="F8">
-        <v>10784896704.219383</v>
-      </c>
-      <c r="G8">
-        <v>35.458238134848095</v>
-      </c>
-      <c r="H8">
-        <v>35.26734159215561</v>
-      </c>
-      <c r="I8">
-        <v>11.227535573950105</v>
-      </c>
-      <c r="J8">
-        <v>1.0291592446967921</v>
-      </c>
-      <c r="K8">
-        <v>39.998500617030622</v>
-      </c>
-      <c r="L8">
-        <v>25.0441175460994</v>
-      </c>
-      <c r="M8">
-        <v>103.21750311087098</v>
-      </c>
-      <c r="N8">
-        <v>35.320773438636586</v>
-      </c>
-      <c r="O8">
-        <v>-6.9202824218865526</v>
-      </c>
-      <c r="P8">
-        <v>37.394201405106315</v>
-      </c>
-      <c r="Q8">
-        <v>6.422533260982461</v>
-      </c>
-      <c r="R8">
-        <v>28.194582095621172</v>
-      </c>
-      <c r="S8">
         <v>16.791435597158287</v>
+      </c>
+      <c r="T7">
+        <v>35.90160013449028</v>
+      </c>
+      <c r="U7">
+        <v>38.804027926164885</v>
       </c>
     </row>
   </sheetData>
@@ -9538,15 +9649,15 @@
     </row>
     <row r="28" spans="6:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F28" s="39"/>
-      <c r="G28" s="93" t="s">
+      <c r="G28" s="97" t="s">
         <v>82</v>
       </c>
-      <c r="H28" s="94"/>
-      <c r="I28" s="94"/>
-      <c r="J28" s="94"/>
-      <c r="K28" s="94"/>
-      <c r="L28" s="94"/>
-      <c r="M28" s="95"/>
+      <c r="H28" s="98"/>
+      <c r="I28" s="98"/>
+      <c r="J28" s="98"/>
+      <c r="K28" s="98"/>
+      <c r="L28" s="98"/>
+      <c r="M28" s="99"/>
     </row>
     <row r="29" spans="6:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F29" s="40" t="s">

</xml_diff>